<commit_message>
Revisado el formato del campo "Coste" de la pestaña "Descarga proyectos" del Informe de costes, ya que aparecian carácteres raros en excel.Cambio de formato de columna coste de excel para que soporte sumatorios.
</commit_message>
<xml_diff>
--- a/GCS/war/datadocs/templateCoste.xlsx
+++ b/GCS/war/datadocs/templateCoste.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="17400" windowHeight="5730" tabRatio="643" activeTab="2"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="17400" windowHeight="5730" tabRatio="643" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Total año Negocio" sheetId="15" r:id="rId1"/>
@@ -246,6 +246,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.00_ ;\-0.00\ "/>
+  </numFmts>
   <fonts count="14">
     <font>
       <sz val="10"/>
@@ -254,6 +257,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -515,7 +519,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -605,6 +609,10 @@
     <xf numFmtId="0" fontId="10" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -670,8 +678,8 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.20445761765197021"/>
-          <c:y val="0.29105726170846336"/>
-          <c:w val="0.51201624930183209"/>
+          <c:y val="0.29105726170846352"/>
+          <c:w val="0.51201624930183176"/>
           <c:h val="0.51704125573504678"/>
         </c:manualLayout>
       </c:layout>
@@ -705,7 +713,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="8.2962273059670993E-2"/>
-                  <c:y val="-2.3735178552800898E-2"/>
+                  <c:y val="-2.3735178552800915E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="bestFit"/>
@@ -790,7 +798,7 @@
           <c:x val="0.11232876712328767"/>
           <c:y val="0.83045138253067263"/>
           <c:w val="0.72602739726027465"/>
-          <c:h val="0.13148812793749637"/>
+          <c:h val="0.13148812793749648"/>
         </c:manualLayout>
       </c:layout>
       <c:txPr>
@@ -833,7 +841,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -870,7 +878,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.16657773360854158"/>
+          <c:x val="0.1665777336085415"/>
           <c:y val="1.7241379310344827E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -893,8 +901,8 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.20445761765197021"/>
-          <c:y val="0.29105726170846336"/>
-          <c:w val="0.51201624930183209"/>
+          <c:y val="0.29105726170846352"/>
+          <c:w val="0.51201624930183176"/>
           <c:h val="0.51704125573504678"/>
         </c:manualLayout>
       </c:layout>
@@ -1000,9 +1008,9 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.11232882297479796"/>
-          <c:y val="0.83044982698962011"/>
-          <c:w val="0.72602731697372846"/>
+          <c:x val="0.11232882297479795"/>
+          <c:y val="0.83044982698962044"/>
+          <c:w val="0.72602731697372891"/>
           <c:h val="0.13148788927335642"/>
         </c:manualLayout>
       </c:layout>
@@ -1046,7 +1054,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1098,8 +1106,8 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.23370866418301481"/>
-          <c:y val="0.26648057003700576"/>
-          <c:w val="0.52665127339939899"/>
+          <c:y val="0.26648057003700604"/>
+          <c:w val="0.52665127339939966"/>
           <c:h val="0.53696999439812665"/>
         </c:manualLayout>
       </c:layout>
@@ -1201,7 +1209,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.11780827153887317"/>
           <c:y val="0.82422047244094565"/>
-          <c:w val="0.71753484697907932"/>
+          <c:w val="0.71753484697907965"/>
           <c:h val="0.16320137569010773"/>
         </c:manualLayout>
       </c:layout>
@@ -1245,7 +1253,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1299,7 +1307,7 @@
           <c:x val="0.22639590255025371"/>
           <c:y val="0.28838782043127098"/>
           <c:w val="0.50471298850111357"/>
-          <c:h val="0.51506274400385987"/>
+          <c:h val="0.51506274400385943"/>
         </c:manualLayout>
       </c:layout>
       <c:pie3DChart>
@@ -1444,7 +1452,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1501,7 +1509,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.18243757753407491"/>
           <c:y val="0.24666550993131742"/>
-          <c:w val="0.74615176449468623"/>
+          <c:w val="0.74615176449468656"/>
           <c:h val="0.40923303553493129"/>
         </c:manualLayout>
       </c:layout>
@@ -1566,11 +1574,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="49034368"/>
-        <c:axId val="49035904"/>
+        <c:axId val="100105600"/>
+        <c:axId val="100279424"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="49034368"/>
+        <c:axId val="100105600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1594,14 +1602,14 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="49035904"/>
+        <c:crossAx val="100279424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="800"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="49035904"/>
+        <c:axId val="100279424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1626,7 +1634,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="49034368"/>
+        <c:crossAx val="100105600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="200"/>
@@ -1654,7 +1662,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2606,8 +2614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:W1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2709,8 +2717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -2718,7 +2726,8 @@
     <col min="1" max="4" width="20" style="20" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" style="20" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="30" style="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="20" style="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20" style="34" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="20" style="20" bestFit="1" customWidth="1"/>
     <col min="11" max="16" width="30" style="20" bestFit="1" customWidth="1"/>
     <col min="17" max="16384" width="9.140625" style="20"/>
   </cols>
@@ -2745,7 +2754,7 @@
       <c r="G1" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="33" t="s">
         <v>27</v>
       </c>
       <c r="I1" s="21" t="s">
@@ -2776,5 +2785,6 @@
   </sheetData>
   <autoFilter ref="A1:P1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
template coste añadiendo control_presupuestario
</commit_message>
<xml_diff>
--- a/GCS/war/datadocs/templateCoste.xlsx
+++ b/GCS/war/datadocs/templateCoste.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="17400" windowHeight="5730" tabRatio="643" activeTab="3"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="17400" windowHeight="5730" tabRatio="643" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Total año Negocio" sheetId="15" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="63">
   <si>
     <t>HORAS</t>
   </si>
@@ -240,6 +240,9 @@
   </si>
   <si>
     <t>FECHA RECEPCION VALORACION</t>
+  </si>
+  <si>
+    <t>CONTROL PRESUPUESTARIO</t>
   </si>
 </sst>
 </file>
@@ -247,7 +250,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.00_ ;\-0.00\ "/>
+    <numFmt numFmtId="164" formatCode="0.00_ ;\-0.00\ "/>
   </numFmts>
   <fonts count="14">
     <font>
@@ -609,10 +612,10 @@
     <xf numFmtId="0" fontId="10" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -678,8 +681,8 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.20445761765197021"/>
-          <c:y val="0.29105726170846352"/>
-          <c:w val="0.51201624930183176"/>
+          <c:y val="0.29105726170846358"/>
+          <c:w val="0.51201624930183165"/>
           <c:h val="0.51704125573504678"/>
         </c:manualLayout>
       </c:layout>
@@ -713,7 +716,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="8.2962273059670993E-2"/>
-                  <c:y val="-2.3735178552800915E-2"/>
+                  <c:y val="-2.3735178552800919E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="bestFit"/>
@@ -798,7 +801,7 @@
           <c:x val="0.11232876712328767"/>
           <c:y val="0.83045138253067263"/>
           <c:w val="0.72602739726027465"/>
-          <c:h val="0.13148812793749648"/>
+          <c:h val="0.13148812793749651"/>
         </c:manualLayout>
       </c:layout>
       <c:txPr>
@@ -841,7 +844,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -878,7 +881,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.1665777336085415"/>
+          <c:x val="0.16657773360854147"/>
           <c:y val="1.7241379310344827E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -901,8 +904,8 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.20445761765197021"/>
-          <c:y val="0.29105726170846352"/>
-          <c:w val="0.51201624930183176"/>
+          <c:y val="0.29105726170846358"/>
+          <c:w val="0.51201624930183165"/>
           <c:h val="0.51704125573504678"/>
         </c:manualLayout>
       </c:layout>
@@ -1009,8 +1012,8 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.11232882297479795"/>
-          <c:y val="0.83044982698962044"/>
-          <c:w val="0.72602731697372891"/>
+          <c:y val="0.83044982698962055"/>
+          <c:w val="0.72602731697372902"/>
           <c:h val="0.13148788927335642"/>
         </c:manualLayout>
       </c:layout>
@@ -1054,7 +1057,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1106,8 +1109,8 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.23370866418301481"/>
-          <c:y val="0.26648057003700604"/>
-          <c:w val="0.52665127339939966"/>
+          <c:y val="0.26648057003700615"/>
+          <c:w val="0.52665127339939988"/>
           <c:h val="0.53696999439812665"/>
         </c:manualLayout>
       </c:layout>
@@ -1253,7 +1256,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1307,7 +1310,7 @@
           <c:x val="0.22639590255025371"/>
           <c:y val="0.28838782043127098"/>
           <c:w val="0.50471298850111357"/>
-          <c:h val="0.51506274400385943"/>
+          <c:h val="0.51506274400385932"/>
         </c:manualLayout>
       </c:layout>
       <c:pie3DChart>
@@ -1452,7 +1455,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1509,7 +1512,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.18243757753407491"/>
           <c:y val="0.24666550993131742"/>
-          <c:w val="0.74615176449468656"/>
+          <c:w val="0.74615176449468679"/>
           <c:h val="0.40923303553493129"/>
         </c:manualLayout>
       </c:layout>
@@ -1574,11 +1577,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="100105600"/>
-        <c:axId val="100279424"/>
+        <c:axId val="53812608"/>
+        <c:axId val="53847168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="100105600"/>
+        <c:axId val="53812608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1602,14 +1605,14 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="100279424"/>
+        <c:crossAx val="53847168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="800"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="100279424"/>
+        <c:axId val="53847168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1634,7 +1637,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="100105600"/>
+        <c:crossAx val="53812608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="200"/>
@@ -1662,7 +1665,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1839,16 +1842,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:W1048576" totalsRowShown="0" tableBorderDxfId="0">
-  <autoFilter ref="A1:W1048576">
-    <filterColumn colId="22"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:X1048576" totalsRowShown="0" tableBorderDxfId="0">
+  <autoFilter ref="A1:X1048576">
+    <filterColumn colId="5"/>
+    <filterColumn colId="23"/>
   </autoFilter>
-  <tableColumns count="23">
+  <tableColumns count="24">
     <tableColumn id="1" name="TIPO"/>
     <tableColumn id="2" name="CLIENTE"/>
     <tableColumn id="3" name="NOMBRE PROYECTO"/>
     <tableColumn id="4" name="NUM. CONTROL"/>
     <tableColumn id="5" name="EQUIPO"/>
+    <tableColumn id="24" name="CONTROL PRESUPUESTARIO"/>
     <tableColumn id="6" name="FECHA ALTA COSTES"/>
     <tableColumn id="7" name="GESTOR IT"/>
     <tableColumn id="8" name="NUM. VALORACION"/>
@@ -2612,10 +2617,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W1"/>
+  <dimension ref="A1:X1"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2623,16 +2628,17 @@
     <col min="2" max="2" width="9.42578125" customWidth="1"/>
     <col min="3" max="3" width="18.28515625" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" customWidth="1"/>
-    <col min="10" max="10" width="27.42578125" customWidth="1"/>
-    <col min="11" max="11" width="27.5703125" customWidth="1"/>
-    <col min="12" max="22" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" customWidth="1"/>
+    <col min="11" max="11" width="27.42578125" customWidth="1"/>
+    <col min="12" max="12" width="27.5703125" customWidth="1"/>
+    <col min="13" max="23" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="23" customFormat="1" ht="22.5" customHeight="1">
+    <row r="1" spans="1:24" s="23" customFormat="1" ht="22.5" customHeight="1">
       <c r="A1" s="24" t="s">
         <v>25</v>
       </c>
@@ -2649,57 +2655,60 @@
         <v>20</v>
       </c>
       <c r="F1" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="H1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="I1" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="25" t="s">
+      <c r="J1" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="26" t="s">
+      <c r="K1" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="26" t="s">
+      <c r="L1" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="L1" s="29" t="s">
+      <c r="M1" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="M1" s="29" t="s">
+      <c r="N1" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="N1" s="27" t="s">
+      <c r="O1" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="O1" s="28" t="s">
+      <c r="P1" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="P1" s="30" t="s">
+      <c r="Q1" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="Q1" s="31" t="s">
+      <c r="R1" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="R1" s="27" t="s">
+      <c r="S1" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="S1" s="28" t="s">
+      <c r="T1" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="T1" s="30" t="s">
+      <c r="U1" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="U1" s="31" t="s">
+      <c r="V1" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="V1" s="32" t="s">
+      <c r="W1" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="W1" s="32" t="s">
+      <c r="X1" s="32" t="s">
         <v>48</v>
       </c>
     </row>
@@ -2717,8 +2726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>

</xml_diff>

<commit_message>
Se mete en la entidad COSTE del CRM los siguientes campos: "Tipo Coste" ,"Asunto","Plazo Entrega Estimado". Se meten nuevos controles de selección de combos
</commit_message>
<xml_diff>
--- a/GCS/war/datadocs/templateCoste.xlsx
+++ b/GCS/war/datadocs/templateCoste.xlsx
@@ -10,11 +10,7 @@
     <sheet name="Total año Negocio" sheetId="15" r:id="rId1"/>
     <sheet name="Total año GSC" sheetId="14" r:id="rId2"/>
     <sheet name="Descarga CRM" sheetId="18" r:id="rId3"/>
-    <sheet name="Descarga proyectos" sheetId="17" r:id="rId4"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Descarga proyectos'!$A$1:$P$1</definedName>
-  </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
@@ -54,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="50">
   <si>
     <t>HORAS</t>
   </si>
@@ -137,46 +133,7 @@
     <t>Lorena Álvarez López</t>
   </si>
   <si>
-    <t>COSTE</t>
-  </si>
-  <si>
     <t>Solutions</t>
-  </si>
-  <si>
-    <t>FECHA ALTA</t>
-  </si>
-  <si>
-    <t>COD. PROYECTO</t>
-  </si>
-  <si>
-    <t>CLASIFICACION</t>
-  </si>
-  <si>
-    <t>GESTOR NEGOCIO</t>
-  </si>
-  <si>
-    <t>PRODUCTO</t>
-  </si>
-  <si>
-    <t>CONECTIVIDAD</t>
-  </si>
-  <si>
-    <t>FECHA INICIO VALORACION</t>
-  </si>
-  <si>
-    <t>FECHA FIN VALORACION</t>
-  </si>
-  <si>
-    <t>FECHA INICIO VIABILIDAD</t>
-  </si>
-  <si>
-    <t>FECHA FIN VIABILIDAD</t>
-  </si>
-  <si>
-    <t>FECHA ENVIO C100</t>
-  </si>
-  <si>
-    <t>FECHA OK NEGOCIO</t>
   </si>
   <si>
     <t>Implementación</t>
@@ -249,10 +206,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.00_ ;\-0.00\ "/>
-  </numFmts>
-  <fonts count="14">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -307,12 +261,6 @@
       <color indexed="56"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="9"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
     <font>
       <b/>
@@ -403,7 +351,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -438,21 +386,6 @@
       </top>
       <bottom style="thin">
         <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
       </bottom>
       <diagonal/>
     </border>
@@ -522,7 +455,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -575,47 +508,39 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -681,8 +606,8 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.20445761765197021"/>
-          <c:y val="0.29105726170846358"/>
-          <c:w val="0.51201624930183165"/>
+          <c:y val="0.29105726170846363"/>
+          <c:w val="0.51201624930183143"/>
           <c:h val="0.51704125573504678"/>
         </c:manualLayout>
       </c:layout>
@@ -716,7 +641,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="8.2962273059670993E-2"/>
-                  <c:y val="-2.3735178552800919E-2"/>
+                  <c:y val="-2.3735178552800926E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="bestFit"/>
@@ -801,7 +726,7 @@
           <c:x val="0.11232876712328767"/>
           <c:y val="0.83045138253067263"/>
           <c:w val="0.72602739726027465"/>
-          <c:h val="0.13148812793749651"/>
+          <c:h val="0.13148812793749654"/>
         </c:manualLayout>
       </c:layout>
       <c:txPr>
@@ -844,7 +769,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -881,7 +806,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.16657773360854147"/>
+          <c:x val="0.16657773360854145"/>
           <c:y val="1.7241379310344827E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -904,8 +829,8 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.20445761765197021"/>
-          <c:y val="0.29105726170846358"/>
-          <c:w val="0.51201624930183165"/>
+          <c:y val="0.29105726170846363"/>
+          <c:w val="0.51201624930183143"/>
           <c:h val="0.51704125573504678"/>
         </c:manualLayout>
       </c:layout>
@@ -1012,8 +937,8 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.11232882297479795"/>
-          <c:y val="0.83044982698962055"/>
-          <c:w val="0.72602731697372902"/>
+          <c:y val="0.83044982698962067"/>
+          <c:w val="0.72602731697372913"/>
           <c:h val="0.13148788927335642"/>
         </c:manualLayout>
       </c:layout>
@@ -1057,7 +982,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1109,8 +1034,8 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.23370866418301481"/>
-          <c:y val="0.26648057003700615"/>
-          <c:w val="0.52665127339939988"/>
+          <c:y val="0.26648057003700626"/>
+          <c:w val="0.5266512733994001"/>
           <c:h val="0.53696999439812665"/>
         </c:manualLayout>
       </c:layout>
@@ -1256,7 +1181,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1310,7 +1235,7 @@
           <c:x val="0.22639590255025371"/>
           <c:y val="0.28838782043127098"/>
           <c:w val="0.50471298850111357"/>
-          <c:h val="0.51506274400385932"/>
+          <c:h val="0.51506274400385921"/>
         </c:manualLayout>
       </c:layout>
       <c:pie3DChart>
@@ -1455,7 +1380,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1512,7 +1437,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.18243757753407491"/>
           <c:y val="0.24666550993131742"/>
-          <c:w val="0.74615176449468679"/>
+          <c:w val="0.7461517644946869"/>
           <c:h val="0.40923303553493129"/>
         </c:manualLayout>
       </c:layout>
@@ -1577,11 +1502,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="53812608"/>
-        <c:axId val="53847168"/>
+        <c:axId val="105933056"/>
+        <c:axId val="105959424"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="53812608"/>
+        <c:axId val="105933056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1605,14 +1530,14 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53847168"/>
+        <c:crossAx val="105959424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="800"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="53847168"/>
+        <c:axId val="105959424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1637,7 +1562,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53812608"/>
+        <c:crossAx val="105933056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="200"/>
@@ -1665,7 +1590,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2186,10 +2111,10 @@
         <v>4</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="2:7" hidden="1">
@@ -2205,18 +2130,18 @@
     </row>
     <row r="4" spans="2:7" hidden="1">
       <c r="E4" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="2:7" hidden="1">
       <c r="E5" s="1" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>26</v>
@@ -2227,7 +2152,7 @@
     </row>
     <row r="6" spans="2:7" hidden="1">
       <c r="E6" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>2</v>
@@ -2235,11 +2160,11 @@
     </row>
     <row r="7" spans="2:7" hidden="1">
       <c r="E7" s="17" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="2:7" hidden="1">
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="20" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2279,25 +2204,25 @@
     </row>
     <row r="14" spans="2:7" ht="20.25" customHeight="1">
       <c r="B14" s="9" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C14" s="4"/>
     </row>
     <row r="15" spans="2:7" ht="20.25" customHeight="1">
       <c r="B15" s="9" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C15" s="4"/>
     </row>
     <row r="16" spans="2:7" ht="20.25" customHeight="1">
       <c r="B16" s="9" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="C16" s="4"/>
     </row>
     <row r="17" spans="2:4" ht="20.25" customHeight="1">
       <c r="B17" s="9" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="8"/>
@@ -2353,7 +2278,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="2:7" hidden="1">
@@ -2369,18 +2294,18 @@
     </row>
     <row r="4" spans="2:7" ht="15" hidden="1" customHeight="1">
       <c r="E4" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="15" hidden="1" customHeight="1">
       <c r="E5" s="1" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>26</v>
@@ -2391,7 +2316,7 @@
     </row>
     <row r="6" spans="2:7" hidden="1">
       <c r="E6" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>2</v>
@@ -2399,14 +2324,14 @@
     </row>
     <row r="7" spans="2:7" hidden="1">
       <c r="E7" s="1" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="2:7" hidden="1">
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="20" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2445,28 +2370,28 @@
     </row>
     <row r="15" spans="2:7" ht="18" customHeight="1">
       <c r="B15" s="9" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C15" s="4"/>
       <c r="E15" s="4"/>
     </row>
     <row r="16" spans="2:7" ht="18" customHeight="1">
       <c r="B16" s="9" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C16" s="4"/>
       <c r="E16" s="4"/>
     </row>
     <row r="17" spans="2:5" ht="18" customHeight="1">
       <c r="B17" s="9" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="C17" s="4"/>
       <c r="E17" s="4"/>
     </row>
     <row r="18" spans="2:5" ht="18" customHeight="1">
       <c r="B18" s="9" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="C18" s="4"/>
       <c r="E18" s="4"/>
@@ -2513,28 +2438,28 @@
     </row>
     <row r="28" spans="2:5" ht="20.25" customHeight="1">
       <c r="B28" s="15" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C28" s="4"/>
       <c r="E28" s="4"/>
     </row>
     <row r="29" spans="2:5" ht="20.25" customHeight="1">
       <c r="B29" s="15" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C29" s="4"/>
       <c r="E29" s="4"/>
     </row>
     <row r="30" spans="2:5" ht="20.25" customHeight="1">
       <c r="B30" s="15" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="C30" s="4"/>
       <c r="E30" s="4"/>
     </row>
     <row r="31" spans="2:5" ht="20.25" customHeight="1">
       <c r="B31" s="15" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="C31" s="4"/>
       <c r="E31" s="4"/>
@@ -2578,28 +2503,28 @@
     </row>
     <row r="42" spans="2:5" ht="18.75" customHeight="1">
       <c r="B42" s="14" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C42" s="4"/>
       <c r="E42" s="4"/>
     </row>
     <row r="43" spans="2:5" ht="18.75" customHeight="1">
       <c r="B43" s="14" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C43" s="4"/>
       <c r="E43" s="4"/>
     </row>
     <row r="44" spans="2:5" ht="18.75" customHeight="1">
       <c r="B44" s="14" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="C44" s="4"/>
       <c r="E44" s="4"/>
     </row>
     <row r="45" spans="2:5" ht="18.75" customHeight="1">
       <c r="B45" s="14" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="C45" s="4"/>
       <c r="E45" s="4"/>
@@ -2638,78 +2563,78 @@
     <col min="13" max="23" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="23" customFormat="1" ht="22.5" customHeight="1">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:24" s="21" customFormat="1" ht="22.5" customHeight="1">
+      <c r="A1" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="G1" s="25" t="s">
+      <c r="F1" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="25" t="s">
+      <c r="I1" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="25" t="s">
+      <c r="J1" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="26" t="s">
+      <c r="K1" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="M1" s="29" t="s">
-        <v>51</v>
-      </c>
-      <c r="N1" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="O1" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="P1" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q1" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="R1" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="S1" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="T1" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="U1" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="V1" s="31" t="s">
-        <v>60</v>
-      </c>
-      <c r="W1" s="32" t="s">
+      <c r="L1" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="M1" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="N1" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="O1" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="P1" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q1" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="R1" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="S1" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="T1" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="U1" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="V1" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="X1" s="32" t="s">
-        <v>48</v>
+      <c r="W1" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="X1" s="30" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -2720,80 +2645,4 @@
     <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
-  <cols>
-    <col min="1" max="4" width="20" style="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="30" style="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20" style="34" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="20" style="20" bestFit="1" customWidth="1"/>
-    <col min="11" max="16" width="30" style="20" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="20"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16" ht="45" customHeight="1">
-      <c r="A1" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="H1" s="33" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="J1" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="K1" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="L1" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="M1" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="N1" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="O1" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="P1" s="21" t="s">
-        <v>40</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:P1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>